<commit_message>
Commiting Conga Templates -> ActualTreatment
</commit_message>
<xml_diff>
--- a/src/resources/Juno_TestDataSheet.xlsx
+++ b/src/resources/Juno_TestDataSheet.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AB074BB7-051C-401F-A8D2-C3686E32DDB2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12653"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterTestDataSheet" sheetId="1" r:id="rId1"/>
     <sheet name="MasterCaseCreation" sheetId="22" r:id="rId2"/>
+    <sheet name="CongaTemplateCreation" sheetId="23" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="179017" calcOnSave="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>Row_ID</t>
   </si>
@@ -46,12 +48,6 @@
     <t>TC_NonPrescriber</t>
   </si>
   <si>
-    <t>..\\Juno_Automation\src\resources\\Juno_TestDataSheet.xlsx</t>
-  </si>
-  <si>
-    <t>https://juno--r3qa.lightning.force.com/one/one.app#/home</t>
-  </si>
-  <si>
     <t>ADMIN_Username</t>
   </si>
   <si>
@@ -62,13 +58,53 @@
   </si>
   <si>
     <t>Agn560102$hsr</t>
+  </si>
+  <si>
+    <t>App</t>
+  </si>
+  <si>
+    <t>Conga Templates</t>
+  </si>
+  <si>
+    <t>TC_CongaTemplates_ActualTreatment</t>
+  </si>
+  <si>
+    <t>CongaTemplateCreation</t>
+  </si>
+  <si>
+    <t>https://test.salesforce.com/</t>
+  </si>
+  <si>
+    <t>..\\JunoAutomation\src\resources\\Juno_TestDataSheet.xlsx</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Auto</t>
+  </si>
+  <si>
+    <t>AutoTueJan081532152019</t>
+  </si>
+  <si>
+    <t>Auto_TueJan081543492019</t>
+  </si>
+  <si>
+    <t>Auto_TueJan081544372019</t>
+  </si>
+  <si>
+    <t>Auto_TueJan081552232019</t>
+  </si>
+  <si>
+    <t>Auto_TueJan081557572019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,7 +201,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -442,23 +478,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.86328125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="45.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.6328125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.81640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.36328125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="45.81640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6328125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +511,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="39.4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -483,93 +519,103 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="7"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -582,40 +628,97 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.36328125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C4B5807-7713-4B6A-BBD1-8485B896927C}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.1796875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="E1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="C2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
         <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
committing non prescriber test case
</commit_message>
<xml_diff>
--- a/src/resources/Juno_TestDataSheet.xlsx
+++ b/src/resources/Juno_TestDataSheet.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12653"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12653" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MasterTestDataSheet" sheetId="1" r:id="rId1"/>
-    <sheet name="MasterCaseCreation" sheetId="22" r:id="rId2"/>
+    <sheet name="MasterDataCreation" sheetId="22" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Row_ID</t>
   </si>
@@ -40,15 +40,9 @@
     <t>GoogleChrome</t>
   </si>
   <si>
-    <t>MasterCaseCreation</t>
-  </si>
-  <si>
     <t>TC_NonPrescriber</t>
   </si>
   <si>
-    <t>..\\Juno_Automation\src\resources\\Juno_TestDataSheet.xlsx</t>
-  </si>
-  <si>
     <t>https://juno--r3qa.lightning.force.com/one/one.app#/home</t>
   </si>
   <si>
@@ -62,6 +56,33 @@
   </si>
   <si>
     <t>Agn560102$hsr</t>
+  </si>
+  <si>
+    <t>App</t>
+  </si>
+  <si>
+    <t>JAMS</t>
+  </si>
+  <si>
+    <t>NonPrescriber</t>
+  </si>
+  <si>
+    <t>Organisation</t>
+  </si>
+  <si>
+    <t>..\\JunoAutomation\src\resources\\Juno_TestDataSheet.xlsx</t>
+  </si>
+  <si>
+    <t>MasterDataCreation</t>
+  </si>
+  <si>
+    <t>Auto_TueJan081543172019</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Auto_TueJan0815431720975</t>
   </si>
 </sst>
 </file>
@@ -445,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -477,16 +498,16 @@
     </row>
     <row r="2" spans="1:5" ht="39.4" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>5</v>
@@ -583,39 +604,65 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="23.3984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing Conga Template - 2
</commit_message>
<xml_diff>
--- a/src/resources/Juno_TestDataSheet.xlsx
+++ b/src/resources/Juno_TestDataSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7F3B5605-B071-4842-BEE2-1CC6CE88BD51}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6A05DAF9-25B7-4683-81E4-64B5AF95EEBF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,7 +14,7 @@
   </sheets>
   <calcPr calcId="179017" calcOnSave="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
   <si>
     <t>Row_ID</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Auto_TueJan081557572019</t>
-  </si>
-  <si>
     <t>MasterDataCreation</t>
   </si>
   <si>
@@ -96,21 +93,26 @@
     <t>JAMS</t>
   </si>
   <si>
-    <t>Auto_TueJan081543172019</t>
-  </si>
-  <si>
     <t>Auto_TueJan0815431720975</t>
   </si>
   <si>
-    <t>Auto_TueJan081751142019</t>
+    <t>Auto_TueJan081816082019</t>
+  </si>
+  <si>
+    <t>Auto_TueJan081846362019</t>
+  </si>
+  <si>
+    <t>TC_CongaTemplates_ProductOrder</t>
+  </si>
+  <si>
+    <t>TC_CongaTemplates_ShipmentAuthorisation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,16 +490,16 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B5" sqref="B5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.6328125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.81640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="21.36328125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="45.81640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6328125" collapsed="true"/>
+    <col min="1" max="1" width="26.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.81640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="45.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.6328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -522,7 +524,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>15</v>
@@ -551,19 +553,39 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+    <row r="4" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
@@ -643,12 +665,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.90625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="5.26953125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.90625" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="24.90625" collapsed="false"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="5.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24.90625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -665,13 +687,13 @@
         <v>11</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -685,16 +707,16 @@
         <v>10</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
         <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -712,11 +734,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.90625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.1796875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="23.90625" collapsed="false"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.90625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -750,7 +772,7 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing 4 object types
</commit_message>
<xml_diff>
--- a/src/resources/Juno_TestDataSheet.xlsx
+++ b/src/resources/Juno_TestDataSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6A05DAF9-25B7-4683-81E4-64B5AF95EEBF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3F60748C-A101-4084-8CCE-A26C96ECD0A2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,7 +14,7 @@
   </sheets>
   <calcPr calcId="179017" calcOnSave="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
   <si>
     <t>Row_ID</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Auto_TueJan0815431720975</t>
   </si>
   <si>
-    <t>Auto_TueJan081816082019</t>
-  </si>
-  <si>
     <t>Auto_TueJan081846362019</t>
   </si>
   <si>
@@ -106,13 +103,44 @@
   </si>
   <si>
     <t>TC_CongaTemplates_ShipmentAuthorisation</t>
+  </si>
+  <si>
+    <t>Auto_TueJan082259102019</t>
+  </si>
+  <si>
+    <t>TC_CongaTemplates_MNCCollectionProcedureRecord</t>
+  </si>
+  <si>
+    <t>Auto_TueJan082325032019</t>
+  </si>
+  <si>
+    <t>Auto_TueJan082328422019</t>
+  </si>
+  <si>
+    <t>Auto_WedJan091057072019</t>
+  </si>
+  <si>
+    <t>Auto_WedJan091058372019</t>
+  </si>
+  <si>
+    <t>Auto_WedJan091059302019</t>
+  </si>
+  <si>
+    <t>Auto_WedJan091101112019</t>
+  </si>
+  <si>
+    <t>Auto_WedJan091102492019</t>
+  </si>
+  <si>
+    <t>Auto_WedJan091104242019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,16 +518,16 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.81640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="45.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.6328125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.81640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.36328125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="45.81640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -555,7 +583,7 @@
     </row>
     <row r="4" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>14</v>
@@ -572,7 +600,7 @@
     </row>
     <row r="5" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>14</v>
@@ -587,12 +615,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="7"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+    <row r="6" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
@@ -665,12 +703,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="5.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="5.26953125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.90625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="24.90625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -710,10 +748,10 @@
         <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
         <v>23</v>
@@ -734,11 +772,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.1796875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.90625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -772,7 +810,7 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commiting latest code Dept,Aph,SiteCreation
</commit_message>
<xml_diff>
--- a/src/resources/Juno_TestDataSheet.xlsx
+++ b/src/resources/Juno_TestDataSheet.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3F60748C-A101-4084-8CCE-A26C96ECD0A2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12653" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MasterTestDataSheet" sheetId="1" r:id="rId1"/>
     <sheet name="MasterDataCreation" sheetId="22" r:id="rId2"/>
     <sheet name="CongaTemplateCreation" sheetId="23" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017" calcOnSave="0"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
   <si>
     <t>Row_ID</t>
   </si>
@@ -90,55 +89,112 @@
     <t>Site</t>
   </si>
   <si>
+    <t>TC_CongaTemplates_ProductOrder</t>
+  </si>
+  <si>
+    <t>TC_CongaTemplates_ShipmentAuthorisation</t>
+  </si>
+  <si>
+    <t>TC_CongaTemplates_MNCCollectionProcedureRecord</t>
+  </si>
+  <si>
+    <t>Auto_WedJan091104242019</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Auto_Address</t>
+  </si>
+  <si>
+    <t>Auto_City</t>
+  </si>
+  <si>
+    <t>Super_Username</t>
+  </si>
+  <si>
+    <t>Super_Password</t>
+  </si>
+  <si>
+    <t>juptrsuperuser@juno.jist.r3qa</t>
+  </si>
+  <si>
+    <t>Testuser2!</t>
+  </si>
+  <si>
+    <t>Auto_WedJan091317342019</t>
+  </si>
+  <si>
+    <t>TC_SiteCreation</t>
+  </si>
+  <si>
+    <t>Accounts</t>
+  </si>
+  <si>
     <t>JAMS</t>
   </si>
   <si>
-    <t>Auto_TueJan0815431720975</t>
-  </si>
-  <si>
-    <t>Auto_TueJan081846362019</t>
-  </si>
-  <si>
-    <t>TC_CongaTemplates_ProductOrder</t>
-  </si>
-  <si>
-    <t>TC_CongaTemplates_ShipmentAuthorisation</t>
-  </si>
-  <si>
-    <t>Auto_TueJan082259102019</t>
-  </si>
-  <si>
-    <t>TC_CongaTemplates_MNCCollectionProcedureRecord</t>
-  </si>
-  <si>
-    <t>Auto_TueJan082325032019</t>
-  </si>
-  <si>
-    <t>Auto_TueJan082328422019</t>
-  </si>
-  <si>
-    <t>Auto_WedJan091057072019</t>
-  </si>
-  <si>
-    <t>Auto_WedJan091058372019</t>
-  </si>
-  <si>
-    <t>Auto_WedJan091059302019</t>
-  </si>
-  <si>
-    <t>Auto_WedJan091101112019</t>
-  </si>
-  <si>
-    <t>Auto_WedJan091102492019</t>
-  </si>
-  <si>
-    <t>Auto_WedJan091104242019</t>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>TC_DepartmentCreation</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>APP_Product</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>App_JAMS</t>
+  </si>
+  <si>
+    <t>APP_JUPTR</t>
+  </si>
+  <si>
+    <t>JuPTR+</t>
+  </si>
+  <si>
+    <t>TC_ProductCreation</t>
+  </si>
+  <si>
+    <t>Auto_WedJan092300162019</t>
+  </si>
+  <si>
+    <t>Auto_WedJan092305192019</t>
+  </si>
+  <si>
+    <t>Auto_WedJan092314402019</t>
+  </si>
+  <si>
+    <t>TC_ProtocolCreation</t>
+  </si>
+  <si>
+    <t>APP_Protocols</t>
+  </si>
+  <si>
+    <t>Protocols</t>
+  </si>
+  <si>
+    <t>Protocol</t>
+  </si>
+  <si>
+    <t>A_Prtcl_ThuJan100113452019</t>
+  </si>
+  <si>
+    <t>Auto_ThuJan101209582019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
   <fonts count="5">
     <font>
@@ -237,7 +293,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -514,23 +570,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.6328125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.81640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="21.36328125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="45.81640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6328125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.59765625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.796875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="45.796875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.59765625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,7 +603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -564,7 +620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -581,9 +637,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>14</v>
@@ -598,9 +654,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>14</v>
@@ -615,9 +671,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>14</v>
@@ -632,56 +688,96 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="7"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="7"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="7"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="7"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="7"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="7"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="7"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="7"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -694,67 +790,143 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.90625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="5.26953125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.90625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="24.90625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.73046875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.9296875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.265625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.3984375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="5.265625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="23.9296875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="24.9296875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.19921875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="8.86328125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="24.1328125" collapsed="false"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="11.265625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="24.1328125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.46484375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="L1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
+      <c r="F2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -763,23 +935,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C4B5807-7713-4B6A-BBD1-8485B896927C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.90625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.1796875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="23.90625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.73046875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.9296875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.19921875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.9296875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -796,7 +968,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -810,7 +982,7 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing merged Excel data sheet
</commit_message>
<xml_diff>
--- a/src/resources/Juno_TestDataSheet.xlsx
+++ b/src/resources/Juno_TestDataSheet.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5F024950-B77E-480B-A039-A7EEBEF0ABE7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12653" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterTestDataSheet" sheetId="1" r:id="rId1"/>
     <sheet name="MasterDataCreation" sheetId="22" r:id="rId2"/>
     <sheet name="CongaTemplateCreation" sheetId="23" r:id="rId3"/>
+    <sheet name="PatientEnrollmentCreation" sheetId="25" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="179017" calcOnSave="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="67">
   <si>
     <t>Row_ID</t>
   </si>
@@ -89,6 +91,9 @@
     <t>Site</t>
   </si>
   <si>
+    <t>JAMS</t>
+  </si>
+  <si>
     <t>TC_CongaTemplates_ProductOrder</t>
   </si>
   <si>
@@ -98,7 +103,76 @@
     <t>TC_CongaTemplates_MNCCollectionProcedureRecord</t>
   </si>
   <si>
-    <t>Auto_WedJan091104242019</t>
+    <t>Super_Username</t>
+  </si>
+  <si>
+    <t>Super_Password</t>
+  </si>
+  <si>
+    <t>juptrsuperuser@juno.jist.r3qa</t>
+  </si>
+  <si>
+    <t>Testuser2!</t>
+  </si>
+  <si>
+    <t>TC_Patient_Enrollment_Approval</t>
+  </si>
+  <si>
+    <t>PatientEnrollmentCreation</t>
+  </si>
+  <si>
+    <t>Patients</t>
+  </si>
+  <si>
+    <t>PAT</t>
+  </si>
+  <si>
+    <t>SubjectNum</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>FName</t>
+  </si>
+  <si>
+    <t>LName</t>
+  </si>
+  <si>
+    <t>EnrollmentNum</t>
+  </si>
+  <si>
+    <t>Auto_ThuJan101154042019</t>
+  </si>
+  <si>
+    <t>ENR-001225</t>
+  </si>
+  <si>
+    <t>App_J</t>
+  </si>
+  <si>
+    <t>JuPTR+</t>
+  </si>
+  <si>
+    <t>Auto_ThuJan101214032019</t>
+  </si>
+  <si>
+    <t>TC_SiteCreation</t>
+  </si>
+  <si>
+    <t>TC_DepartmentCreation</t>
+  </si>
+  <si>
+    <t>TC_ProductCreation</t>
+  </si>
+  <si>
+    <t>TC_ProtocolCreation</t>
+  </si>
+  <si>
+    <t>App_JAMS</t>
+  </si>
+  <si>
+    <t>APP_JUPTR</t>
   </si>
   <si>
     <t>Address</t>
@@ -107,96 +181,56 @@
     <t>City</t>
   </si>
   <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>APP_Product</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>APP_Protocols</t>
+  </si>
+  <si>
+    <t>Protocol</t>
+  </si>
+  <si>
+    <t>Accounts</t>
+  </si>
+  <si>
+    <t>Auto_WedJan091317342019</t>
+  </si>
+  <si>
+    <t>Auto_WedJan092314402019</t>
+  </si>
+  <si>
     <t>Auto_Address</t>
   </si>
   <si>
     <t>Auto_City</t>
   </si>
   <si>
-    <t>Super_Username</t>
-  </si>
-  <si>
-    <t>Super_Password</t>
-  </si>
-  <si>
-    <t>juptrsuperuser@juno.jist.r3qa</t>
-  </si>
-  <si>
-    <t>Testuser2!</t>
-  </si>
-  <si>
-    <t>Auto_WedJan091317342019</t>
-  </si>
-  <si>
-    <t>TC_SiteCreation</t>
-  </si>
-  <si>
-    <t>Accounts</t>
-  </si>
-  <si>
-    <t>JAMS</t>
-  </si>
-  <si>
-    <t>Department</t>
-  </si>
-  <si>
-    <t>TC_DepartmentCreation</t>
-  </si>
-  <si>
-    <t>Product</t>
-  </si>
-  <si>
-    <t>APP_Product</t>
+    <t>Auto_ThuJan101209582019</t>
   </si>
   <si>
     <t>Products</t>
   </si>
   <si>
-    <t>App_JAMS</t>
-  </si>
-  <si>
-    <t>APP_JUPTR</t>
-  </si>
-  <si>
-    <t>JuPTR+</t>
-  </si>
-  <si>
-    <t>TC_ProductCreation</t>
-  </si>
-  <si>
     <t>Auto_WedJan092300162019</t>
   </si>
   <si>
-    <t>Auto_WedJan092305192019</t>
-  </si>
-  <si>
-    <t>Auto_WedJan092314402019</t>
-  </si>
-  <si>
-    <t>TC_ProtocolCreation</t>
-  </si>
-  <si>
-    <t>APP_Protocols</t>
-  </si>
-  <si>
     <t>Protocols</t>
   </si>
   <si>
-    <t>Protocol</t>
-  </si>
-  <si>
     <t>A_Prtcl_ThuJan100113452019</t>
-  </si>
-  <si>
-    <t>Auto_ThuJan101209582019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,7 +327,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -570,23 +604,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.59765625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.796875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="21.33203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="45.796875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.59765625" collapsed="true"/>
+    <col min="1" max="1" width="26.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.81640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="45.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.6328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,7 +637,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -620,7 +654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -637,9 +671,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>14</v>
@@ -654,9 +688,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>14</v>
@@ -671,9 +705,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>14</v>
@@ -688,12 +722,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>15</v>
@@ -705,9 +739,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>18</v>
@@ -722,9 +756,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>18</v>
@@ -739,9 +773,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>18</v>
@@ -756,28 +790,38 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="7"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="7"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -790,42 +834,43 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="23.73046875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.9296875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.265625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.3984375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="5.265625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="23.9296875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="24.9296875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.19921875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="8.86328125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="24.1328125" collapsed="false"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="11.265625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="24.1328125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.46484375" collapsed="true"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="5.26953125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="23.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="24.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="24.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="25.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>7</v>
@@ -837,10 +882,10 @@
         <v>11</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>19</v>
@@ -852,36 +897,36 @@
         <v>21</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>9</v>
@@ -890,43 +935,43 @@
         <v>10</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I2" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="K2" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="M2" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="N2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="O2" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="P2" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="Q2" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="R2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -935,57 +980,182 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C4B5807-7713-4B6A-BBD1-8485B896927C}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.73046875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.9296875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.19921875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="23.9296875" collapsed="true"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.90625" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="H1" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{77C35B00-B477-4CA9-9F54-D1A7931AE8F6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{139D3D1B-E3E6-4589-B8D4-BFB850EB1C57}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.7265625" customWidth="1"/>
+    <col min="5" max="5" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="C1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="K1" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
+      <c r="K2" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{5EC1AC83-5D68-44A9-9CA6-C1CA29754E16}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
committing merging ot PAT_ENR_Creation
</commit_message>
<xml_diff>
--- a/src/resources/Juno_TestDataSheet.xlsx
+++ b/src/resources/Juno_TestDataSheet.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E4F47F7E-16DD-4080-9C05-56995E4055B6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12653"/>
   </bookViews>
   <sheets>
     <sheet name="MasterTestDataSheet" sheetId="1" r:id="rId1"/>
@@ -13,9 +12,9 @@
     <sheet name="CongaTemplateCreation" sheetId="23" r:id="rId3"/>
     <sheet name="PatientEnrollmentCreation" sheetId="25" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179017" calcOnSave="0"/>
+  <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="98">
   <si>
     <t>Row_ID</t>
   </si>
@@ -190,12 +189,6 @@
     <t>Accounts</t>
   </si>
   <si>
-    <t>Auto_WedJan091317342019</t>
-  </si>
-  <si>
-    <t>Auto_WedJan092314402019</t>
-  </si>
-  <si>
     <t>Auto_Address</t>
   </si>
   <si>
@@ -205,15 +198,9 @@
     <t>Products</t>
   </si>
   <si>
-    <t>Auto_WedJan092300162019</t>
-  </si>
-  <si>
     <t>Protocols</t>
   </si>
   <si>
-    <t>A_Prtcl_ThuJan100113452019</t>
-  </si>
-  <si>
     <t>TC_ReservationTreatment_ActualTreatment</t>
   </si>
   <si>
@@ -223,9 +210,6 @@
     <t>Treatments</t>
   </si>
   <si>
-    <t>AThuJan101939562019</t>
-  </si>
-  <si>
     <t>ENR-001231</t>
   </si>
   <si>
@@ -256,9 +240,6 @@
     <t>APP_ProductVersion</t>
   </si>
   <si>
-    <t>Auto_ThuJan101444302019</t>
-  </si>
-  <si>
     <t>AutomationOTAPh</t>
   </si>
   <si>
@@ -308,13 +289,41 @@
   </si>
   <si>
     <t>A_DS_ThuJan171728172019</t>
+  </si>
+  <si>
+    <t>A_NonPresc_ThuJan171813322019</t>
+  </si>
+  <si>
+    <t>A_Org_ThuJan171813322019</t>
+  </si>
+  <si>
+    <t>A_Site_ThuJan171816342019</t>
+  </si>
+  <si>
+    <t>AThuJan171820582019</t>
+  </si>
+  <si>
+    <t>A_Prdct_ThuJan171825202019</t>
+  </si>
+  <si>
+    <t>A_Prtcl_ThuJan171828292019</t>
+  </si>
+  <si>
+    <t>AThuJan171836332019</t>
+  </si>
+  <si>
+    <t>AThuJan171845542019</t>
+  </si>
+  <si>
+    <t>AFriJan181104062019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,7 +420,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -688,23 +697,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="26.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.81640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="45.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.59765625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.796875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="45.796875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.59765625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -721,7 +730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -738,7 +747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -755,7 +764,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -772,7 +781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
@@ -789,7 +798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>25</v>
       </c>
@@ -806,12 +815,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>15</v>
@@ -823,7 +832,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>41</v>
       </c>
@@ -840,7 +849,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
         <v>42</v>
       </c>
@@ -857,7 +866,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="7" t="s">
         <v>43</v>
       </c>
@@ -874,7 +883,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="7" t="s">
         <v>44</v>
       </c>
@@ -891,9 +900,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A12" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>31</v>
@@ -908,9 +917,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A13" s="7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>31</v>
@@ -925,9 +934,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A14" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>18</v>
@@ -942,9 +951,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>18</v>
@@ -959,9 +968,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>18</v>
@@ -976,9 +985,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>18</v>
@@ -999,43 +1008,43 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AA2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.26953125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="23.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="24.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="24.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="25.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="23.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="23.1796875" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="26.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="23.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.59765625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.73046875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.9296875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.265625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.33203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.86328125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="23.9296875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="24.9296875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.19921875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="8.796875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="24.06640625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="11.265625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="24.06640625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.46484375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="25.9296875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="18.19921875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="23.19921875" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="23.19921875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="26.06640625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="10.19921875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="23.73046875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="13.46484375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="23.796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1091,34 +1100,61 @@
         <v>53</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="W1" s="5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="AA1" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1144,61 +1180,88 @@
         <v>40</v>
       </c>
       <c r="I2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K2" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" t="s">
         <v>55</v>
       </c>
-      <c r="J2" t="s">
-        <v>55</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>56</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
+        <v>92</v>
+      </c>
+      <c r="O2" t="s">
         <v>57</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q2" t="s">
         <v>58</v>
       </c>
-      <c r="N2" t="s">
-        <v>77</v>
-      </c>
-      <c r="O2" t="s">
-        <v>59</v>
-      </c>
-      <c r="P2" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
+        <v>94</v>
+      </c>
+      <c r="S2" t="s">
+        <v>82</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="U2" t="s">
+        <v>83</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="W2" t="s">
+        <v>84</v>
+      </c>
+      <c r="X2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC2" t="s">
         <v>61</v>
       </c>
-      <c r="R2" t="s">
+      <c r="AD2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ2" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="S2" t="s">
-        <v>88</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="U2" t="s">
-        <v>89</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="W2" t="s">
-        <v>90</v>
-      </c>
-      <c r="X2" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1207,26 +1270,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C4B5807-7713-4B6A-BBD1-8485B896927C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.90625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.33203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.9296875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.9296875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.19921875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.9296875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="23.73046875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.9296875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1252,7 +1315,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1269,7 +1332,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>9</v>
@@ -1280,38 +1343,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{77C35B00-B477-4CA9-9F54-D1A7931AE8F6}"/>
+    <hyperlink ref="B2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{139D3D1B-E3E6-4589-B8D4-BFB850EB1C57}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="E1" sqref="E1:M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.7265625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.1796875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.1796875" customWidth="1"/>
-    <col min="8" max="8" width="24.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.33203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.73046875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.73046875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.19921875" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="15.19921875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="24.73046875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="23.73046875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.796875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.73046875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.9296875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="14.06640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1328,10 +1390,10 @@
         <v>11</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>36</v>
@@ -1352,7 +1414,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1369,16 +1431,16 @@
         <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
         <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>35</v>
@@ -1390,12 +1452,12 @@
         <v>10</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{5EC1AC83-5D68-44A9-9CA6-C1CA29754E16}"/>
+    <hyperlink ref="B2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
committing PV manual join Aprroval
</commit_message>
<xml_diff>
--- a/src/resources/Juno_TestDataSheet.xlsx
+++ b/src/resources/Juno_TestDataSheet.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1B9A0E5F-16F1-4F6C-9AF3-2C1FE313ECCA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12653" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterTestDataSheet" sheetId="1" r:id="rId1"/>
@@ -12,9 +13,9 @@
     <sheet name="CongaTemplateCreation" sheetId="23" r:id="rId3"/>
     <sheet name="PatientEnrollmentCreation" sheetId="25" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="179017" calcOnSave="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="110">
   <si>
     <t>Row_ID</t>
   </si>
@@ -328,13 +329,38 @@
   </si>
   <si>
     <t>A_PVMJ_FriJan181345582019</t>
+  </si>
+  <si>
+    <t>Join Name</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>AFriJan181534322019</t>
+  </si>
+  <si>
+    <t>A_PVMJ_FriJan181536322019</t>
+  </si>
+  <si>
+    <t>A_PVMJ_FriJan181543152019</t>
+  </si>
+  <si>
+    <t>A_PVMJ_FriJan181550122019</t>
+  </si>
+  <si>
+    <t>A_PVMJ_FriJan181634082019</t>
+  </si>
+  <si>
+    <t>A_PVMJ_FriJan181641252019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,7 +471,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -722,23 +748,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.796875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="45.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.6328125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.81640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.36328125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="45.81640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6328125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -755,7 +781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -772,7 +798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -789,7 +815,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -806,7 +832,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
@@ -823,7 +849,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>25</v>
       </c>
@@ -840,7 +866,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>30</v>
       </c>
@@ -857,7 +883,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>41</v>
       </c>
@@ -874,7 +900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>42</v>
       </c>
@@ -891,7 +917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>43</v>
       </c>
@@ -908,7 +934,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>44</v>
       </c>
@@ -925,7 +951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>59</v>
       </c>
@@ -942,7 +968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>75</v>
       </c>
@@ -959,7 +985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>65</v>
       </c>
@@ -976,7 +1002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>66</v>
       </c>
@@ -993,7 +1019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>67</v>
       </c>
@@ -1010,7 +1036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>76</v>
       </c>
@@ -1027,7 +1053,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>92</v>
       </c>
@@ -1050,46 +1076,47 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AM2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AK4" sqref="AK4"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL5" sqref="AL5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.9296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="23.9296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.9296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="8.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="24.06640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="24.06640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.46484375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="25.9296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="18.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="23.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="23.19921875" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="26.06640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="10.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="23.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="13.46484375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="23.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="14.06640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="33.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="25.06640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.6328125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.90625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.26953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.36328125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.81640625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="23.90625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="24.90625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.1796875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="8.81640625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="24.08984375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="11.26953125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="24.08984375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="25.90625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="18.1796875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="23.1796875" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="23.1796875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="26.08984375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="23.81640625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="15.90625" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="14.08984375" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="33.36328125" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="25.08984375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1204,8 +1231,11 @@
       <c r="AL1" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.45">
+      <c r="AM1" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1318,7 +1348,10 @@
         <v>100</v>
       </c>
       <c r="AL2" t="s">
-        <v>101</v>
+        <v>108</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1327,26 +1360,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.9296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.9296875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.9296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.9296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.36328125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.90625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.90625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.1796875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.90625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.90625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1372,7 +1405,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1389,7 +1422,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>9</v>
@@ -1400,37 +1433,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.73046875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="15.19921875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.9296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.06640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.36328125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.7265625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.7265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.1796875" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="15.1796875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="24.7265625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.90625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="14.08984375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1471,7 +1504,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1514,7 +1547,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Committing total suite with 18 testcases.
</commit_message>
<xml_diff>
--- a/src/resources/Juno_TestDataSheet.xlsx
+++ b/src/resources/Juno_TestDataSheet.xlsx
@@ -14,7 +14,7 @@
   </sheets>
   <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="117">
   <si>
     <t>Row_ID</t>
   </si>
@@ -117,9 +117,6 @@
     <t>TC_Patient_Enrollment_Approval</t>
   </si>
   <si>
-    <t>PatientEnrollmentCreation</t>
-  </si>
-  <si>
     <t>Patients</t>
   </si>
   <si>
@@ -285,81 +282,104 @@
     <t>ProductVersionManulJoin</t>
   </si>
   <si>
-    <t>AutomationManufacturingSite</t>
-  </si>
-  <si>
     <t>Manufacturing Schedule Configuration</t>
   </si>
   <si>
     <t>Join Name</t>
   </si>
   <si>
-    <t>A_PVMJ_FriJan181641252019</t>
-  </si>
-  <si>
     <t>AMonJan211116562019</t>
   </si>
   <si>
-    <t>A_PVMJ_MonJan211124592019</t>
-  </si>
-  <si>
-    <t>A_NonPresc_MonJan211141582019</t>
-  </si>
-  <si>
-    <t>A_Org_MonJan211141582019</t>
-  </si>
-  <si>
-    <t>A_Site_MonJan211158372019</t>
-  </si>
-  <si>
-    <t>AMonJan211204302019</t>
-  </si>
-  <si>
-    <t>A_Prdct_MonJan211210452019</t>
-  </si>
-  <si>
-    <t>A_Prtcl_MonJan211213582019</t>
-  </si>
-  <si>
     <t>App_Patients</t>
   </si>
   <si>
-    <t>AMonJan211241382019</t>
-  </si>
-  <si>
-    <t>ENR-001234</t>
-  </si>
-  <si>
-    <t>A_Aph_MonJan211255272019</t>
-  </si>
-  <si>
-    <t>A_PVAJ_MonJan211452592019</t>
-  </si>
-  <si>
-    <t>A_DL_MonJan211452592019</t>
-  </si>
-  <si>
-    <t>A_DS_MonJan211452592019</t>
-  </si>
-  <si>
-    <t>A_PVAJ_MonJan211511192019</t>
-  </si>
-  <si>
-    <t>A_DL_MonJan211511192019</t>
-  </si>
-  <si>
-    <t>A_DS_MonJan211511192019</t>
-  </si>
-  <si>
-    <t>A_Aph_MonJan211726342019</t>
+    <t>A_NonPresc_221805402019</t>
+  </si>
+  <si>
+    <t>A_Org_221805402019</t>
+  </si>
+  <si>
+    <t>A_Site_221807452019</t>
+  </si>
+  <si>
+    <t>ATueJan221814022019</t>
+  </si>
+  <si>
+    <t>A_Prdct_221818242019</t>
+  </si>
+  <si>
+    <t>A_Prtcl_221822232019</t>
+  </si>
+  <si>
+    <t>OnboardingID</t>
+  </si>
+  <si>
+    <t>A_MS_231113102019</t>
+  </si>
+  <si>
+    <t>A_PVAJ_231132032019</t>
+  </si>
+  <si>
+    <t>A_DL_231132042019</t>
+  </si>
+  <si>
+    <t>A_DS_231132042019</t>
+  </si>
+  <si>
+    <t>Verifier</t>
+  </si>
+  <si>
+    <t>Vaibhav Agnihotri</t>
+  </si>
+  <si>
+    <t>TC_TRT_DL_DS_Status</t>
+  </si>
+  <si>
+    <t>TreatmentCreated</t>
+  </si>
+  <si>
+    <t>A_PVMJ_241320202019</t>
+  </si>
+  <si>
+    <t>A_PVMJ_241326462019</t>
+  </si>
+  <si>
+    <t>AThuJan241455102019</t>
+  </si>
+  <si>
+    <t>ENR-001238</t>
+  </si>
+  <si>
+    <t>TC_ApheresisOnboardingTemplate</t>
+  </si>
+  <si>
+    <t>AphOnboardingTemplate</t>
+  </si>
+  <si>
+    <t>Onboarding Templates</t>
+  </si>
+  <si>
+    <t>App_OnboardingTemplate</t>
+  </si>
+  <si>
+    <t>A_AOBT_ThuJan241558102019</t>
+  </si>
+  <si>
+    <t>A_Aph_241834492019</t>
+  </si>
+  <si>
+    <t>OB-000188</t>
+  </si>
+  <si>
+    <t>TRT-007772</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,7 +428,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -429,17 +449,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -464,9 +473,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,19 +755,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.59765625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.796875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="21.33203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="45.796875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.59765625" collapsed="true"/>
+    <col min="1" max="1" width="26.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.796875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="45.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.59765625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
@@ -797,131 +804,131 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
+      <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="7" t="s">
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+      <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>15</v>
@@ -935,7 +942,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="7" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>18</v>
@@ -952,10 +959,10 @@
     </row>
     <row r="12" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A12" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>15</v>
@@ -969,10 +976,10 @@
     </row>
     <row r="13" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A13" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>15</v>
@@ -986,7 +993,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>18</v>
@@ -1003,7 +1010,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>18</v>
@@ -1020,7 +1027,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>18</v>
@@ -1037,7 +1044,7 @@
     </row>
     <row r="17" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>18</v>
@@ -1053,8 +1060,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A18" s="8" t="s">
-        <v>84</v>
+      <c r="A18" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>18</v>
@@ -1066,6 +1073,40 @@
         <v>16</v>
       </c>
       <c r="E18" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1076,46 +1117,55 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM2"/>
+  <dimension ref="A1:AU2"/>
   <sheetViews>
-    <sheetView zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView topLeftCell="AN1" zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AQ14" sqref="AQ14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="24.59765625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="23.73046875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.9296875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.265625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.33203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="9.796875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="23.9296875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="24.9296875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.19921875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="8.796875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="24.06640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="11.265625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="24.06640625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="12.46484375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="25.9296875" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="18.19921875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="23.19921875" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="23.19921875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="26.06640625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="10.19921875" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="23.73046875" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="13.46484375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="23.796875" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="15.9296875" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="14.06640625" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="33.33203125" collapsed="true"/>
-    <col min="38" max="39" bestFit="true" customWidth="true" width="25.06640625" collapsed="true"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.9296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="23.9296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="24.9296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="8.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="24.06640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="24.06640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.46484375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="25.9296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="24.9296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="18.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="18.19921875" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="23.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="23.19921875" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="26.06640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="10.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="23.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="13.46484375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="23.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="14.06640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="33.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="39" width="25.06640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="14.46484375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="14.9296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="15.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="22.46484375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="26.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1135,10 +1185,10 @@
         <v>11</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>19</v>
@@ -1150,91 +1200,115 @@
         <v>21</v>
       </c>
       <c r="L1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="R1" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="S1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="T1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="V1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="V1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="AA1" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB1" s="5" t="s">
-        <v>99</v>
-      </c>
       <c r="AC1" s="5" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="AD1" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AE1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AH1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AG1" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="AH1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ1" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="AK1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL1" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="AL1" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="AM1" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.45">
+        <v>87</v>
+      </c>
+      <c r="AN1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AR1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AS1" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AT1" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AU1" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1251,106 +1325,130 @@
         <v>10</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>22</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" t="s">
         <v>93</v>
       </c>
-      <c r="J2" t="s">
+      <c r="O2" t="s">
+        <v>56</v>
+      </c>
+      <c r="P2" t="s">
         <v>94</v>
       </c>
-      <c r="K2" t="s">
+      <c r="Q2" t="s">
+        <v>57</v>
+      </c>
+      <c r="R2" t="s">
         <v>95</v>
       </c>
-      <c r="L2" t="s">
-        <v>55</v>
-      </c>
-      <c r="M2" t="s">
-        <v>56</v>
-      </c>
-      <c r="N2" t="s">
-        <v>96</v>
-      </c>
-      <c r="O2" t="s">
-        <v>57</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="S2" t="s">
+        <v>114</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="V2" t="s">
         <v>97</v>
       </c>
-      <c r="Q2" t="s">
-        <v>58</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="W2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="X2" t="s">
         <v>98</v>
       </c>
-      <c r="S2" t="s">
-        <v>109</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="U2" t="s">
-        <v>87</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AJ2" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="AK2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AM2" t="s">
         <v>106</v>
       </c>
-      <c r="X2" t="s">
-        <v>81</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>107</v>
-      </c>
-      <c r="Z2" t="s">
+      <c r="AN2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ2" t="s">
         <v>82</v>
       </c>
-      <c r="AA2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AG2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="AI2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="AJ2" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="AK2" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>90</v>
+      <c r="AR2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1363,19 +1461,19 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="26.33203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.9296875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.9296875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.19921875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="23.9296875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="23.73046875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="15.9296875" collapsed="true"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.9296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.9296875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.9296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.9296875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
@@ -1389,7 +1487,7 @@
         <v>27</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>11</v>
@@ -1415,13 +1513,13 @@
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>9</v>
@@ -1432,7 +1530,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1442,24 +1540,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H13:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="26.33203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.73046875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.73046875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.19921875" collapsed="true"/>
-    <col min="6" max="7" customWidth="true" width="15.19921875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="24.73046875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="23.73046875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.796875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="23.73046875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="15.9296875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="14.06640625" collapsed="true"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.73046875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.19921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="15.19921875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="24.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.9296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.06640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.45">
@@ -1473,25 +1571,25 @@
         <v>27</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="J1" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>7</v>
@@ -1500,7 +1598,7 @@
         <v>8</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.45">
@@ -1514,25 +1612,25 @@
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" t="s">
-        <v>33</v>
-      </c>
       <c r="I2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>9</v>
@@ -1541,12 +1639,12 @@
         <v>10</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId5"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Committing after suite run
</commit_message>
<xml_diff>
--- a/src/resources/Juno_TestDataSheet.xlsx
+++ b/src/resources/Juno_TestDataSheet.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{26F338CF-9F61-499D-8E05-7650EEF732AC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12653"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterTestDataSheet" sheetId="1" r:id="rId1"/>
@@ -12,9 +13,9 @@
     <sheet name="CongaTemplateCreation" sheetId="23" r:id="rId3"/>
     <sheet name="PatientEnrollmentCreation" sheetId="25" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" calcOnSave="0"/>
+  <calcPr calcId="179017" calcOnSave="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="168">
   <si>
     <t>Row_ID</t>
   </si>
@@ -288,30 +289,9 @@
     <t>Join Name</t>
   </si>
   <si>
-    <t>AMonJan211116562019</t>
-  </si>
-  <si>
     <t>App_Patients</t>
   </si>
   <si>
-    <t>A_NonPresc_221805402019</t>
-  </si>
-  <si>
-    <t>A_Org_221805402019</t>
-  </si>
-  <si>
-    <t>A_Site_221807452019</t>
-  </si>
-  <si>
-    <t>ATueJan221814022019</t>
-  </si>
-  <si>
-    <t>A_Prdct_221818242019</t>
-  </si>
-  <si>
-    <t>A_Prtcl_221822232019</t>
-  </si>
-  <si>
     <t>OnboardingID</t>
   </si>
   <si>
@@ -345,12 +325,6 @@
     <t>A_PVMJ_241326462019</t>
   </si>
   <si>
-    <t>AThuJan241455102019</t>
-  </si>
-  <si>
-    <t>ENR-001238</t>
-  </si>
-  <si>
     <t>TC_ApheresisOnboardingTemplate</t>
   </si>
   <si>
@@ -373,13 +347,194 @@
   </si>
   <si>
     <t>TRT-007772</t>
+  </si>
+  <si>
+    <t>ATueJan291500452019</t>
+  </si>
+  <si>
+    <t>ATueJan291549522019</t>
+  </si>
+  <si>
+    <t>ENR-001242</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>A_NonPresc_291604062019</t>
+  </si>
+  <si>
+    <t>A_Org_291604072019</t>
+  </si>
+  <si>
+    <t>A_Site_291606162019</t>
+  </si>
+  <si>
+    <t>ATueJan291610322019</t>
+  </si>
+  <si>
+    <t>A_Prdct_291614472019</t>
+  </si>
+  <si>
+    <t>A_Prtcl_291617522019</t>
+  </si>
+  <si>
+    <t>ATueJan291621162019</t>
+  </si>
+  <si>
+    <t>ENR-001243</t>
+  </si>
+  <si>
+    <t>A_AOBT_TueJan291626462019</t>
+  </si>
+  <si>
+    <t>A_Aph_291628272019</t>
+  </si>
+  <si>
+    <t>OB-000189</t>
+  </si>
+  <si>
+    <t>A_MS_291634152019</t>
+  </si>
+  <si>
+    <t>A_PVAJ_291638372019</t>
+  </si>
+  <si>
+    <t>A_DL_291638372019</t>
+  </si>
+  <si>
+    <t>A_DS_291638372019</t>
+  </si>
+  <si>
+    <t>A_AOBT_TueJan291656172019</t>
+  </si>
+  <si>
+    <t>A_Aph_291657592019</t>
+  </si>
+  <si>
+    <t>OB-000190</t>
+  </si>
+  <si>
+    <t>A_MS_291703502019</t>
+  </si>
+  <si>
+    <t>A_AOBT_TueJan291706362019</t>
+  </si>
+  <si>
+    <t>A_Aph_291708362019</t>
+  </si>
+  <si>
+    <t>A_MS_291711132019</t>
+  </si>
+  <si>
+    <t>A_Aph_291713272019</t>
+  </si>
+  <si>
+    <t>OB-000191</t>
+  </si>
+  <si>
+    <t>A_AOBT_TueJan291720102019</t>
+  </si>
+  <si>
+    <t>A_Aph_291721542019</t>
+  </si>
+  <si>
+    <t>A_MS_291724572019</t>
+  </si>
+  <si>
+    <t>A_PVAJ_291729402019</t>
+  </si>
+  <si>
+    <t>A_DL_291729402019</t>
+  </si>
+  <si>
+    <t>A_DS_291729402019</t>
+  </si>
+  <si>
+    <t>A_AOBT_TueJan291820592019</t>
+  </si>
+  <si>
+    <t>A_Aph_291822422019</t>
+  </si>
+  <si>
+    <t>OB-000192</t>
+  </si>
+  <si>
+    <t>A_MS_291828242019</t>
+  </si>
+  <si>
+    <t>A_PVAJ_291832442019</t>
+  </si>
+  <si>
+    <t>A_DL_291832442019</t>
+  </si>
+  <si>
+    <t>A_DS_291832442019</t>
+  </si>
+  <si>
+    <t>A_AOBT_WedJan301137172019</t>
+  </si>
+  <si>
+    <t>A_Aph_301139052019</t>
+  </si>
+  <si>
+    <t>OB-000193</t>
+  </si>
+  <si>
+    <t>A_MS_301145032019</t>
+  </si>
+  <si>
+    <t>A_PVAJ_301149352019</t>
+  </si>
+  <si>
+    <t>A_DL_301149352019</t>
+  </si>
+  <si>
+    <t>A_DS_301149352019</t>
+  </si>
+  <si>
+    <t>A_PVAJ_301206122019</t>
+  </si>
+  <si>
+    <t>A_DL_301206122019</t>
+  </si>
+  <si>
+    <t>A_DS_301206122019</t>
+  </si>
+  <si>
+    <t>A_PVAJ_301215522019</t>
+  </si>
+  <si>
+    <t>A_DL_301215532019</t>
+  </si>
+  <si>
+    <t>A_DS_301215532019</t>
+  </si>
+  <si>
+    <t>AWedJan301224572019</t>
+  </si>
+  <si>
+    <t>AWedJan301229072019</t>
+  </si>
+  <si>
+    <t>AWedJan301230562019</t>
+  </si>
+  <si>
+    <t>AWedJan301232472019</t>
+  </si>
+  <si>
+    <t>A_PVMJ_301234392019</t>
+  </si>
+  <si>
+    <t>A_PVMJ_301241172019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -477,7 +632,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -754,23 +909,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.796875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="45.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.6328125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.81640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.36328125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="45.81640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.6328125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -787,7 +942,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -804,7 +959,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>40</v>
       </c>
@@ -821,7 +976,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>41</v>
       </c>
@@ -838,7 +993,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>42</v>
       </c>
@@ -855,7 +1010,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>43</v>
       </c>
@@ -872,7 +1027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -889,7 +1044,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -906,7 +1061,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -923,7 +1078,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
@@ -940,7 +1095,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>30</v>
       </c>
@@ -957,7 +1112,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>58</v>
       </c>
@@ -974,7 +1129,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>73</v>
       </c>
@@ -991,7 +1146,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>64</v>
       </c>
@@ -1008,7 +1163,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>65</v>
       </c>
@@ -1025,7 +1180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>66</v>
       </c>
@@ -1042,7 +1197,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="26.25" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>74</v>
       </c>
@@ -1059,7 +1214,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>83</v>
       </c>
@@ -1076,9 +1231,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>18</v>
@@ -1093,9 +1248,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>18</v>
@@ -1116,56 +1271,56 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AU2"/>
   <sheetViews>
-    <sheetView topLeftCell="AN1" zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AQ14" sqref="AQ14"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.9296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="23.9296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="24.9296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="8.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="24.06640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="24.06640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.46484375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="25.9296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="24.9296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="18.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="18.19921875" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="23.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="23.19921875" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="26.06640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="10.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="23.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="13.46484375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="23.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="23" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="14.06640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="33.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="39" width="25.06640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="14.46484375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="14.9296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="15.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="22.46484375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="26.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="24.6328125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.90625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.26953125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.36328125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.81640625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="23.6328125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="23.90625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="24.90625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.1796875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="8.81640625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="24.08984375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="11.26953125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="24.08984375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="25.90625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="24.90625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="18.1796875" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="18.1796875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="23.1796875" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="23.1796875" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="26.08984375" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="23.81640625" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="14.08984375" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="33.36328125" collapsed="true"/>
+    <col min="38" max="39" bestFit="true" customWidth="true" width="25.08984375" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="14.90625" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" width="22.453125" collapsed="true"/>
+    <col min="47" max="47" bestFit="true" customWidth="true" width="26.1796875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1227,7 +1382,7 @@
         <v>68</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="V1" s="5" t="s">
         <v>69</v>
@@ -1251,7 +1406,7 @@
         <v>79</v>
       </c>
       <c r="AC1" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD1" s="5" t="s">
         <v>59</v>
@@ -1269,7 +1424,7 @@
         <v>33</v>
       </c>
       <c r="AI1" s="5" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="AJ1" s="5" t="s">
         <v>37</v>
@@ -1299,16 +1454,16 @@
         <v>33</v>
       </c>
       <c r="AS1" s="8" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="AT1" s="8" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="AU1" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.45">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1334,13 +1489,13 @@
         <v>39</v>
       </c>
       <c r="I2" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="J2" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="K2" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="L2" t="s">
         <v>54</v>
@@ -1349,49 +1504,49 @@
         <v>55</v>
       </c>
       <c r="N2" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="O2" t="s">
         <v>56</v>
       </c>
       <c r="P2" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="Q2" t="s">
         <v>57</v>
       </c>
       <c r="R2" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="S2" t="s">
-        <v>114</v>
+        <v>150</v>
       </c>
       <c r="T2" s="6" t="s">
         <v>71</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="V2" t="s">
-        <v>97</v>
+        <v>152</v>
       </c>
       <c r="W2" s="6" t="s">
         <v>72</v>
       </c>
       <c r="X2" t="s">
-        <v>98</v>
+        <v>159</v>
       </c>
       <c r="Y2" t="s">
         <v>80</v>
       </c>
       <c r="Z2" t="s">
-        <v>99</v>
+        <v>160</v>
       </c>
       <c r="AA2" t="s">
         <v>81</v>
       </c>
       <c r="AB2" t="s">
-        <v>100</v>
+        <v>161</v>
       </c>
       <c r="AC2" t="s">
         <v>31</v>
@@ -1406,25 +1561,25 @@
         <v>32</v>
       </c>
       <c r="AG2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="AH2" s="6" t="s">
         <v>34</v>
       </c>
       <c r="AI2" s="6" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="AJ2" s="6" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="AK2" s="6" t="s">
         <v>86</v>
       </c>
       <c r="AL2" t="s">
-        <v>105</v>
+        <v>166</v>
       </c>
       <c r="AM2" t="s">
-        <v>106</v>
+        <v>167</v>
       </c>
       <c r="AN2" t="s">
         <v>60</v>
@@ -1442,13 +1597,13 @@
         <v>34</v>
       </c>
       <c r="AS2" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="AT2" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="AU2" t="s">
-        <v>113</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1457,26 +1612,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.9296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.9296875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.9296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.9296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.36328125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.90625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.90625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.1796875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="23.90625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="15.90625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1502,7 +1657,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1519,7 +1674,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>88</v>
+        <v>165</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>9</v>
@@ -1530,37 +1685,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId57" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="H14" sqref="H13:H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.73046875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.19921875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="15.19921875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.73046875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.9296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.06640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.36328125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.7265625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.7265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.1796875" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="15.1796875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="24.7265625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="15.90625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="14.08984375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1601,7 +1756,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1644,7 +1799,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId57" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>